<commit_message>
add 1 to PKI
</commit_message>
<xml_diff>
--- a/Patching Schedule-2019-03.XLSX
+++ b/Patching Schedule-2019-03.XLSX
@@ -1102,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E29:E30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -1981,7 +1981,9 @@
       <c r="D31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="29">
+        <v>1</v>
+      </c>
       <c r="F31" s="29"/>
       <c r="G31" s="25" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
delete 1; add 2
</commit_message>
<xml_diff>
--- a/Patching Schedule-2019-03.XLSX
+++ b/Patching Schedule-2019-03.XLSX
@@ -1103,7 +1103,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -1981,9 +1981,7 @@
       <c r="D31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="29">
-        <v>1</v>
-      </c>
+      <c r="E31" s="29"/>
       <c r="F31" s="29"/>
       <c r="G31" s="25" t="s">
         <v>105</v>
@@ -2039,7 +2037,9 @@
       <c r="D33" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="36"/>
+      <c r="E33" s="36">
+        <v>2</v>
+      </c>
       <c r="F33" s="36"/>
       <c r="G33" s="25" t="s">
         <v>105</v>

</xml_diff>